<commit_message>
especificacion de hadware y software
</commit_message>
<xml_diff>
--- a/Actividades/Desarrollo/Act3/historias de usuario.xlsx
+++ b/Actividades/Desarrollo/Act3/historias de usuario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Minion\Documents\GitHub\sena\Actividades\Desarrollo\Act3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5840F9BD-B1D2-471B-83B4-3AD8F30A6AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F85DE1F-F9F2-498C-A859-DF6534FAD769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -72,9 +72,6 @@
     <t>Como cliente quiero un cuadro de busqueda para poder filtrar los productos por categorías</t>
   </si>
   <si>
-    <t>Como cliente quiero una opcion de calificación en cada producto  para poder valporarlo</t>
-  </si>
-  <si>
     <t>poder crear un usuario</t>
   </si>
   <si>
@@ -184,6 +181,9 @@
   </si>
   <si>
     <t>Historia de usuario 17:</t>
+  </si>
+  <si>
+    <t>Como cliente quiero una opcion de calificación en cada producto  para poder valorarlo</t>
   </si>
 </sst>
 </file>
@@ -360,8 +360,11 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -369,14 +372,11 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -745,9 +745,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:K20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G20" sqref="G20:H20"/>
+      <selection pane="bottomLeft" activeCell="G6" sqref="G6:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -795,309 +795,286 @@
       <c r="E3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
     </row>
     <row r="4" spans="2:11" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="12"/>
+      <c r="H4" s="9"/>
     </row>
     <row r="5" spans="2:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="9"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="11" t="s">
+      <c r="B5" s="10"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="12"/>
+      <c r="H5" s="9"/>
     </row>
     <row r="6" spans="2:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="9"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="11" t="s">
+      <c r="B6" s="10"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="H6" s="9"/>
+    </row>
+    <row r="7" spans="2:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="12"/>
-    </row>
-    <row r="7" spans="2:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="10" t="s">
+      <c r="G7" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="H7" s="9"/>
+    </row>
+    <row r="8" spans="2:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="10"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="12"/>
-    </row>
-    <row r="8" spans="2:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="9"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="11" t="s">
+      <c r="H8" s="9"/>
+      <c r="K8" s="6"/>
+    </row>
+    <row r="9" spans="2:11" ht="27" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B9" s="10"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G9" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="12"/>
-      <c r="K8" s="6"/>
-    </row>
-    <row r="9" spans="2:11" ht="27" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="H9" s="12"/>
+      <c r="H9" s="9"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
     </row>
     <row r="10" spans="2:11" ht="27" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" s="12"/>
+      <c r="F10" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="9"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
     </row>
     <row r="11" spans="2:11" ht="27" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B11" s="9"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="H11" s="12"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="9"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
     </row>
     <row r="12" spans="2:11" ht="27" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B12" s="9"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="H12" s="12"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="9"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
     </row>
     <row r="13" spans="2:11" ht="27" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B13" s="9"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="H13" s="13"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="12"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
     </row>
     <row r="14" spans="2:11" ht="27" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="9"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="H14" s="13"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" s="12"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
     </row>
     <row r="15" spans="2:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="D15" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="E15" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="F15" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="H15" s="9"/>
+    </row>
+    <row r="16" spans="2:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="10"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="G15" s="12" t="s">
+      <c r="G16" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="H15" s="12"/>
-    </row>
-    <row r="16" spans="2:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="9"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="11" t="s">
+      <c r="H16" s="9"/>
+    </row>
+    <row r="17" spans="2:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="10"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="G16" s="12" t="s">
+      <c r="G17" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="H16" s="12"/>
-    </row>
-    <row r="17" spans="2:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="9"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="11" t="s">
+      <c r="H17" s="9"/>
+    </row>
+    <row r="18" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="10"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="G17" s="12" t="s">
+      <c r="G18" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="H17" s="12"/>
-    </row>
-    <row r="18" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="9"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="11" t="s">
+      <c r="H18" s="9"/>
+    </row>
+    <row r="19" spans="2:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="10"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="G18" s="12" t="s">
+      <c r="G19" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="H18" s="12"/>
-    </row>
-    <row r="19" spans="2:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="9"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="11" t="s">
+      <c r="H19" s="9"/>
+    </row>
+    <row r="20" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="10"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="G19" s="12" t="s">
+      <c r="G20" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="H19" s="12"/>
-    </row>
-    <row r="20" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="9"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="H20" s="12"/>
+      <c r="H20" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="B15:B20"/>
-    <mergeCell ref="C15:C20"/>
-    <mergeCell ref="D15:D20"/>
-    <mergeCell ref="E15:E20"/>
-    <mergeCell ref="D10:D14"/>
-    <mergeCell ref="E10:E14"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="B10:B14"/>
-    <mergeCell ref="C10:C14"/>
     <mergeCell ref="F3:H3"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="G5:H5"/>
@@ -1109,6 +1086,29 @@
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="G8:H8"/>
     <mergeCell ref="G9:H9"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="B10:B14"/>
+    <mergeCell ref="C10:C14"/>
+    <mergeCell ref="D10:D14"/>
+    <mergeCell ref="E10:E14"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="B15:B20"/>
+    <mergeCell ref="C15:C20"/>
+    <mergeCell ref="D15:D20"/>
+    <mergeCell ref="E15:E20"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G19:H19"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>